<commit_message>
Implemented first prototype sorter
Created a sorter that matches schedules and regions of the instructors and the institutions. 
Reads input from excel database, sorts it, and displays it in the terminal.
</commit_message>
<xml_diff>
--- a/schoolsample.xlsx
+++ b/schoolsample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmins\Desktop\DreamsForSchools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC09CE14-8972-4277-8C73-0DEADD0B6F89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1A4C6D-DADD-4B4B-BCEA-B6DA52A60E58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8544" yWindow="-288" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>School Name</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>15:00 - 16:30</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Orange County</t>
+  </si>
+  <si>
+    <t>Riverside</t>
   </si>
 </sst>
 </file>
@@ -508,22 +517,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,19 +541,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -551,19 +564,22 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -571,19 +587,22 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -591,19 +610,22 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -611,19 +633,22 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -631,19 +656,22 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -651,19 +679,22 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -671,19 +702,22 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -691,19 +725,22 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -711,19 +748,22 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -731,19 +771,22 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -751,15 +794,18 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>